<commit_message>
updated to use overlay.html at default landing page
</commit_message>
<xml_diff>
--- a/webconfig/Holocene_Volcanoes_volcdef_cfg.xlsx
+++ b/webconfig/Holocene_Volcanoes_volcdef_cfg.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/famelung/code/minsar/tools/VolcDef_web/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/famelung/code/minsar/webconfig/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F5AC24D-61E9-9647-B03C-2E6A41D3D725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B2DB32-34F2-0845-8162-195EF52A8873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3540" yWindow="660" windowWidth="29500" windowHeight="19160" xr2:uid="{C0385577-DB88-5B46-BC32-5548AF298521}"/>
   </bookViews>
@@ -5978,16 +5978,16 @@
     <t>http://149.165.154.65/data/HDF5EOS/Chiles/mintpy</t>
   </si>
   <si>
-    <t>http://149.165.154.65/data/HDF5EOS/Fernandina/mintpy</t>
-  </si>
-  <si>
-    <t>http://149.165.154.65/data/HDF5EOS/hvGalapagos/mintpy</t>
-  </si>
-  <si>
-    <t>http://149.165.154.65/data/HDF5EOS/Alcedo/miaplpy</t>
-  </si>
-  <si>
-    <t>http://149.165.154.65/data/HDF5EOS/Fernandina/miaplpy</t>
+    <t>http://149.165.154.65/data/HDF5EOS/Fernandina/miaplpy/overlay.html</t>
+  </si>
+  <si>
+    <t>http://149.165.154.65/data/HDF5EOS/Fernandina/mintpy/overlay.html</t>
+  </si>
+  <si>
+    <t>http://149.165.154.65/data/HDF5EOS/Alcedo/miaplpy/overlay.html</t>
+  </si>
+  <si>
+    <t>http://149.165.154.65/data/HDF5EOS/hvGalapagos/mintpy/overlay.html</t>
   </si>
 </sst>
 </file>
@@ -6447,8 +6447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEFAE601-3978-2241-8BCB-1E3D7A07C3BA}">
   <dimension ref="A1:N1327"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1059" workbookViewId="0">
-      <selection activeCell="B1079" sqref="B1079"/>
+    <sheetView tabSelected="1" topLeftCell="A1040" workbookViewId="0">
+      <selection activeCell="B1084" sqref="B1084"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -53830,7 +53830,7 @@
     </row>
     <row r="1078" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1078" s="5" t="s">
-        <v>1983</v>
+        <v>1980</v>
       </c>
       <c r="B1078" s="3">
         <v>353010</v>
@@ -53874,7 +53874,7 @@
     </row>
     <row r="1079" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1079" s="5" t="s">
-        <v>1980</v>
+        <v>1981</v>
       </c>
       <c r="B1079" s="3">
         <v>353010</v>
@@ -54094,7 +54094,7 @@
     </row>
     <row r="1084" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1084" s="5" t="s">
-        <v>1981</v>
+        <v>1983</v>
       </c>
       <c r="B1084" s="3">
         <v>353050</v>

</xml_diff>